<commit_message>
correctie op filter wkt
correctie op scripts omdat ik niet goed had gelezen en dacht dat ik archeologischOnderzoeksgebied MET geometrie (WKT) weg moest filteren. Maar na goed lezen is het juist ZONDER geometrie die weggefilterd mag. dat is hier opgelost
</commit_message>
<xml_diff>
--- a/vergelijking_ldv_vs_archis.xlsx
+++ b/vergelijking_ldv_vs_archis.xlsx
@@ -481,10 +481,10 @@
         <v>97461</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>108969</v>
       </c>
       <c r="F2" t="n">
-        <v>206430</v>
+        <v>97461</v>
       </c>
     </row>
     <row r="3">
@@ -503,10 +503,10 @@
         <v>97461</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>108969</v>
       </c>
       <c r="F3" t="n">
-        <v>206430</v>
+        <v>97461</v>
       </c>
     </row>
     <row r="4">
@@ -679,10 +679,10 @@
         <v>104473</v>
       </c>
       <c r="E11" t="n">
-        <v>218</v>
+        <v>103195</v>
       </c>
       <c r="F11" t="n">
-        <v>207668</v>
+        <v>104691</v>
       </c>
     </row>
     <row r="12">
@@ -877,10 +877,10 @@
         <v>102027</v>
       </c>
       <c r="E20" t="n">
-        <v>125401</v>
+        <v>233909</v>
       </c>
       <c r="F20" t="n">
-        <v>210772</v>
+        <v>102264</v>
       </c>
     </row>
     <row r="21">
@@ -899,10 +899,10 @@
         <v>102027</v>
       </c>
       <c r="E21" t="n">
-        <v>125401</v>
+        <v>233909</v>
       </c>
       <c r="F21" t="n">
-        <v>210772</v>
+        <v>102264</v>
       </c>
     </row>
     <row r="22">
@@ -921,10 +921,10 @@
         <v>72710</v>
       </c>
       <c r="E22" t="n">
-        <v>109395</v>
+        <v>212372</v>
       </c>
       <c r="F22" t="n">
-        <v>175905</v>
+        <v>72928</v>
       </c>
     </row>
     <row r="23">
@@ -943,10 +943,10 @@
         <v>72710</v>
       </c>
       <c r="E23" t="n">
-        <v>109395</v>
+        <v>212372</v>
       </c>
       <c r="F23" t="n">
-        <v>175905</v>
+        <v>72928</v>
       </c>
     </row>
     <row r="24">
@@ -1009,10 +1009,10 @@
         <v>97461</v>
       </c>
       <c r="E26" t="n">
-        <v>0</v>
+        <v>108969</v>
       </c>
       <c r="F26" t="n">
-        <v>206430</v>
+        <v>97461</v>
       </c>
     </row>
     <row r="27">
@@ -1163,10 +1163,10 @@
         <v>212912</v>
       </c>
       <c r="E33" t="n">
-        <v>979970</v>
+        <v>1082947</v>
       </c>
       <c r="F33" t="n">
-        <v>316107</v>
+        <v>213130</v>
       </c>
     </row>
     <row r="34">
@@ -1317,10 +1317,10 @@
         <v>-777867</v>
       </c>
       <c r="E40" t="n">
-        <v>3878005</v>
+        <v>4035911</v>
       </c>
       <c r="F40" t="n">
-        <v>-619495</v>
+        <v>-777401</v>
       </c>
     </row>
     <row r="41">
@@ -1537,10 +1537,10 @@
         <v>97461</v>
       </c>
       <c r="E50" t="n">
-        <v>0</v>
+        <v>108969</v>
       </c>
       <c r="F50" t="n">
-        <v>206430</v>
+        <v>97461</v>
       </c>
     </row>
     <row r="51">
@@ -1559,10 +1559,10 @@
         <v>97461</v>
       </c>
       <c r="E51" t="n">
-        <v>0</v>
+        <v>108969</v>
       </c>
       <c r="F51" t="n">
-        <v>206430</v>
+        <v>97461</v>
       </c>
     </row>
     <row r="52">
@@ -1889,10 +1889,10 @@
         <v>36667</v>
       </c>
       <c r="E66" t="n">
-        <v>21</v>
+        <v>4733</v>
       </c>
       <c r="F66" t="n">
-        <v>41400</v>
+        <v>36688</v>
       </c>
     </row>
     <row r="67">
@@ -1933,10 +1933,10 @@
         <v>437900</v>
       </c>
       <c r="E68" t="n">
-        <v>862129</v>
+        <v>908831</v>
       </c>
       <c r="F68" t="n">
-        <v>484756</v>
+        <v>438054</v>
       </c>
     </row>
     <row r="69">
@@ -1955,10 +1955,10 @@
         <v>437900</v>
       </c>
       <c r="E69" t="n">
-        <v>862129</v>
+        <v>908831</v>
       </c>
       <c r="F69" t="n">
-        <v>484756</v>
+        <v>438054</v>
       </c>
     </row>
     <row r="70">
@@ -2087,10 +2087,10 @@
         <v>-777867</v>
       </c>
       <c r="E75" t="n">
-        <v>3878005</v>
+        <v>4035911</v>
       </c>
       <c r="F75" t="n">
-        <v>-619495</v>
+        <v>-777401</v>
       </c>
     </row>
     <row r="76">
@@ -2109,10 +2109,10 @@
         <v>-777867</v>
       </c>
       <c r="E76" t="n">
-        <v>3878005</v>
+        <v>4035911</v>
       </c>
       <c r="F76" t="n">
-        <v>-619495</v>
+        <v>-777401</v>
       </c>
     </row>
     <row r="77">
@@ -2527,10 +2527,10 @@
         <v>212912</v>
       </c>
       <c r="E95" t="n">
-        <v>979970</v>
+        <v>1082947</v>
       </c>
       <c r="F95" t="n">
-        <v>316107</v>
+        <v>213130</v>
       </c>
     </row>
     <row r="96">
@@ -2571,10 +2571,10 @@
         <v>-240364</v>
       </c>
       <c r="E97" t="n">
-        <v>586510</v>
+        <v>744416</v>
       </c>
       <c r="F97" t="n">
-        <v>-81992</v>
+        <v>-239898</v>
       </c>
     </row>
     <row r="98">
@@ -2593,10 +2593,10 @@
         <v>-240364</v>
       </c>
       <c r="E98" t="n">
-        <v>586510</v>
+        <v>744416</v>
       </c>
       <c r="F98" t="n">
-        <v>-81992</v>
+        <v>-239898</v>
       </c>
     </row>
     <row r="99">
@@ -2725,10 +2725,10 @@
         <v>102027</v>
       </c>
       <c r="E104" t="n">
-        <v>125401</v>
+        <v>233909</v>
       </c>
       <c r="F104" t="n">
-        <v>210772</v>
+        <v>102264</v>
       </c>
     </row>
     <row r="105">
@@ -2769,10 +2769,10 @@
         <v>3652281</v>
       </c>
       <c r="E106" t="n">
-        <v>10332986</v>
+        <v>10798477</v>
       </c>
       <c r="F106" t="n">
-        <v>4119076</v>
+        <v>3653585</v>
       </c>
     </row>
     <row r="107">
@@ -2879,10 +2879,10 @@
         <v>-311590</v>
       </c>
       <c r="E111" t="n">
-        <v>4604610</v>
+        <v>4865493</v>
       </c>
       <c r="F111" t="n">
-        <v>-50023</v>
+        <v>-310906</v>
       </c>
     </row>
     <row r="112">
@@ -2901,10 +2901,10 @@
         <v>875800</v>
       </c>
       <c r="E112" t="n">
-        <v>1771114</v>
+        <v>1817816</v>
       </c>
       <c r="F112" t="n">
-        <v>922656</v>
+        <v>875954</v>
       </c>
     </row>
     <row r="113">
@@ -3011,10 +3011,10 @@
         <v>875800</v>
       </c>
       <c r="E117" t="n">
-        <v>1771114</v>
+        <v>1817816</v>
       </c>
       <c r="F117" t="n">
-        <v>922656</v>
+        <v>875954</v>
       </c>
     </row>
     <row r="118">
@@ -3209,10 +3209,10 @@
         <v>-98538</v>
       </c>
       <c r="E126" t="n">
-        <v>586157</v>
+        <v>615498</v>
       </c>
       <c r="F126" t="n">
-        <v>-69084</v>
+        <v>-98425</v>
       </c>
     </row>
     <row r="127">
@@ -3297,10 +3297,10 @@
         <v>1088712</v>
       </c>
       <c r="E130" t="n">
-        <v>2751084</v>
+        <v>2900763</v>
       </c>
       <c r="F130" t="n">
-        <v>1238763</v>
+        <v>1089084</v>
       </c>
     </row>
     <row r="131">
@@ -3319,10 +3319,10 @@
         <v>-777867</v>
       </c>
       <c r="E131" t="n">
-        <v>3878005</v>
+        <v>4035911</v>
       </c>
       <c r="F131" t="n">
-        <v>-619495</v>
+        <v>-777401</v>
       </c>
     </row>
     <row r="132">
@@ -3385,10 +3385,10 @@
         <v>3652281</v>
       </c>
       <c r="E134" t="n">
-        <v>10332986</v>
+        <v>10798477</v>
       </c>
       <c r="F134" t="n">
-        <v>4119076</v>
+        <v>3653585</v>
       </c>
     </row>
     <row r="135">
@@ -3429,10 +3429,10 @@
         <v>3532984</v>
       </c>
       <c r="E136" t="n">
-        <v>442540</v>
+        <v>703423</v>
       </c>
       <c r="F136" t="n">
-        <v>3794551</v>
+        <v>3533668</v>
       </c>
     </row>
     <row r="137">
@@ -3583,10 +3583,10 @@
         <v>2805403</v>
       </c>
       <c r="E143" t="n">
-        <v>294735</v>
+        <v>452641</v>
       </c>
       <c r="F143" t="n">
-        <v>2963775</v>
+        <v>2805869</v>
       </c>
     </row>
     <row r="144">

</xml_diff>